<commit_message>
updated SCBAA, all line graphs
</commit_message>
<xml_diff>
--- a/SCBAA/2016/ARMM.xlsx
+++ b/SCBAA/2016/ARMM.xlsx
@@ -1,33 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mngx\thesis\SCBA\Done XLSX - 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mngx\thesis\SCBAA\2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B41F58-EF71-4A8E-82D1-C175943EF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BEA277-93BB-4E78-BA93-88056CEE2CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="240" windowWidth="14625" windowHeight="12540" activeTab="2" xr2:uid="{FCCC59F1-88A9-4466-AAB0-E027C4520B94}"/>
+    <workbookView xWindow="12570" yWindow="345" windowWidth="14880" windowHeight="7260" activeTab="1" xr2:uid="{FCCC59F1-88A9-4466-AAB0-E027C4520B94}"/>
   </bookViews>
   <sheets>
     <sheet name="Isabela" sheetId="1" r:id="rId1"/>
     <sheet name="Marawi" sheetId="2" r:id="rId2"/>
     <sheet name="Lamitan" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="67">
   <si>
     <t>TOTAL APPROPRIATIONS</t>
   </si>
@@ -222,9 +229,6 @@
   </si>
   <si>
     <t>CITY OF ISABELA</t>
-  </si>
-  <si>
-    <t>For the Year Ended December 31, 2015</t>
   </si>
   <si>
     <t>CITY OF MARAWI</t>
@@ -588,18 +592,6 @@
     <xf numFmtId="40" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="22" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="40" fontId="22" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -608,23 +600,11 @@
     <xf numFmtId="4" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="4" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="23" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="22" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -654,6 +634,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="22" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="40" fontId="22" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="23" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="22" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -989,54 +993,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
@@ -1050,22 +1054,22 @@
       <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="38" t="s">
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="60" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="39"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="61"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
@@ -1176,7 +1180,7 @@
       <c r="D18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1208,7 +1212,7 @@
         <v>46</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="41">
+      <c r="E21" s="37">
         <v>439112403</v>
       </c>
     </row>
@@ -1219,7 +1223,7 @@
         <v>45</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="41">
+      <c r="E22" s="37">
         <v>269552.82</v>
       </c>
     </row>
@@ -1239,7 +1243,7 @@
       <c r="D24" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="42">
+      <c r="E24" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1261,7 +1265,7 @@
       <c r="D26" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1272,7 +1276,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1303,7 +1307,7 @@
       <c r="D30" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="38">
         <v>0</v>
       </c>
     </row>
@@ -1314,7 +1318,7 @@
         <v>36</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="E31" s="43">
+      <c r="E31" s="39">
         <v>0</v>
       </c>
     </row>
@@ -1334,7 +1338,7 @@
       <c r="D33" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="44">
+      <c r="E33" s="40">
         <v>0</v>
       </c>
     </row>
@@ -1367,7 +1371,7 @@
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="43">
+      <c r="E36" s="39">
         <v>0</v>
       </c>
     </row>
@@ -1424,7 +1428,7 @@
       <c r="D42" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="41">
+      <c r="E42" s="37">
         <v>150502827.58000001</v>
       </c>
     </row>
@@ -1435,7 +1439,7 @@
       <c r="D43" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="41">
+      <c r="E43" s="37">
         <v>123853447</v>
       </c>
       <c r="F43" s="7"/>
@@ -1447,7 +1451,7 @@
       <c r="D44" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E44" s="41">
+      <c r="E44" s="37">
         <v>3220917.74</v>
       </c>
       <c r="F44" s="7"/>
@@ -1511,7 +1515,7 @@
       <c r="D50" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="41">
+      <c r="E50" s="37">
         <f>24506064.18-263813.25</f>
         <v>24242250.93</v>
       </c>
@@ -1523,7 +1527,7 @@
       <c r="D51" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="41">
+      <c r="E51" s="37">
         <v>1920776.23</v>
       </c>
     </row>
@@ -1534,7 +1538,7 @@
       <c r="D52" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E52" s="41">
+      <c r="E52" s="37">
         <v>31390</v>
       </c>
     </row>
@@ -1565,7 +1569,7 @@
       <c r="D55" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="40">
+      <c r="E55" s="36">
         <v>0</v>
       </c>
     </row>
@@ -1576,7 +1580,7 @@
       <c r="D56" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="45">
+      <c r="E56" s="41">
         <v>0</v>
       </c>
     </row>
@@ -1596,7 +1600,7 @@
       <c r="D58" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="44">
+      <c r="E58" s="40">
         <v>0</v>
       </c>
     </row>
@@ -1607,7 +1611,7 @@
       <c r="D59" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E59" s="46">
+      <c r="E59" s="42">
         <v>0</v>
       </c>
     </row>
@@ -1618,7 +1622,7 @@
       <c r="D60" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E60" s="44">
+      <c r="E60" s="40">
         <v>0</v>
       </c>
     </row>
@@ -1638,7 +1642,7 @@
       <c r="D62" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E62" s="41">
+      <c r="E62" s="37">
         <v>4289450.9000000004</v>
       </c>
     </row>
@@ -1649,7 +1653,7 @@
       <c r="D63" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="41">
+      <c r="E63" s="37">
         <v>3030717.39</v>
       </c>
     </row>
@@ -1660,7 +1664,7 @@
       <c r="D64" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E64" s="41">
+      <c r="E64" s="37">
         <v>84940</v>
       </c>
     </row>
@@ -1680,7 +1684,7 @@
       <c r="D66" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="41">
+      <c r="E66" s="37">
         <v>23665846.449999999</v>
       </c>
       <c r="G66" s="7"/>
@@ -1692,7 +1696,7 @@
       <c r="D67" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E67" s="41">
+      <c r="E67" s="37">
         <v>2072231.09</v>
       </c>
       <c r="G67" s="7"/>
@@ -1704,7 +1708,7 @@
       <c r="D68" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E68" s="41">
+      <c r="E68" s="37">
         <v>128816</v>
       </c>
       <c r="G68" s="7"/>
@@ -1776,7 +1780,7 @@
       <c r="D75" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E75" s="41">
+      <c r="E75" s="37">
         <v>6684100.7000000002</v>
       </c>
     </row>
@@ -1787,7 +1791,7 @@
       <c r="D76" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E76" s="47">
+      <c r="E76" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1807,7 +1811,7 @@
       <c r="D78" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E78" s="41">
+      <c r="E78" s="37">
         <f>9030468+5000000</f>
         <v>14030468</v>
       </c>
@@ -1820,7 +1824,7 @@
       <c r="D79" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E79" s="41">
+      <c r="E79" s="37">
         <v>5258132</v>
       </c>
     </row>
@@ -1840,7 +1844,7 @@
       <c r="D81" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E81" s="41">
+      <c r="E81" s="37">
         <v>10482688.439999999</v>
       </c>
       <c r="F81" s="20"/>
@@ -1852,7 +1856,7 @@
       <c r="D82" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E82" s="41">
+      <c r="E82" s="37">
         <v>38915353.649999999</v>
       </c>
       <c r="F82" s="19"/>
@@ -1946,7 +1950,7 @@
       <c r="D91" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E91" s="41">
+      <c r="E91" s="37">
         <f>17272822.5+28305705.15</f>
         <v>45578527.649999999</v>
       </c>
@@ -1958,7 +1962,7 @@
       <c r="D92" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E92" s="45">
+      <c r="E92" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2025,7 +2029,7 @@
       <c r="D98" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E98" s="40">
+      <c r="E98" s="36">
         <v>0</v>
       </c>
     </row>
@@ -2079,7 +2083,7 @@
       <c r="D104" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E104" s="44">
+      <c r="E104" s="40">
         <v>0</v>
       </c>
     </row>
@@ -2178,8 +2182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9EF0239-B27D-4590-8540-2F5B458C0B15}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="E111" sqref="E11:E111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,54 +2201,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="A1" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
+      <c r="A3" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
+      <c r="A4" s="58"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
@@ -2258,22 +2262,22 @@
       <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="38" t="s">
+      <c r="B6" s="58"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="60" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="39"/>
+      <c r="A7" s="58"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="61"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
@@ -2309,7 +2313,7 @@
         <v>56</v>
       </c>
       <c r="E11" s="7">
-        <v>1047828.22</v>
+        <v>0</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -2339,7 +2343,7 @@
         <v>54</v>
       </c>
       <c r="E13" s="7">
-        <v>24500</v>
+        <v>0</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -2355,7 +2359,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="25">
         <f>SUM(E11:E13)</f>
-        <v>1072328.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2375,7 +2379,7 @@
         <v>51</v>
       </c>
       <c r="E16" s="7">
-        <v>306560</v>
+        <v>0</v>
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -2388,7 +2392,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="7">
-        <v>143850</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2399,7 +2403,7 @@
         <v>49</v>
       </c>
       <c r="E18" s="7">
-        <v>61275776.130000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2411,7 +2415,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="25">
         <f>SUM(E16:E18)</f>
-        <v>61726186.130000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2431,7 +2435,7 @@
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="7">
-        <v>428753688</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2461,7 +2465,7 @@
       <c r="D24" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="42">
+      <c r="E24" s="38">
         <v>0</v>
       </c>
     </row>
@@ -2484,7 +2488,7 @@
         <v>41</v>
       </c>
       <c r="E26" s="7">
-        <v>5887266.4800000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2494,7 +2498,7 @@
       <c r="D27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="38">
         <v>0</v>
       </c>
     </row>
@@ -2525,7 +2529,7 @@
       <c r="D30" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="38">
         <v>0</v>
       </c>
     </row>
@@ -2536,7 +2540,7 @@
         <v>36</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="E31" s="43">
+      <c r="E31" s="39">
         <v>0</v>
       </c>
     </row>
@@ -2556,7 +2560,7 @@
       <c r="D33" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="44">
+      <c r="E33" s="40">
         <v>0</v>
       </c>
     </row>
@@ -2589,7 +2593,7 @@
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="43">
+      <c r="E36" s="39">
         <v>0</v>
       </c>
     </row>
@@ -2602,7 +2606,7 @@
       <c r="D37" s="8"/>
       <c r="E37" s="25">
         <f>SUM(E14,E19,E21:E36)</f>
-        <v>497439468.83000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2647,7 +2651,7 @@
         <v>26</v>
       </c>
       <c r="E42" s="7">
-        <v>112881339.08</v>
+        <v>0</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
@@ -2669,7 +2673,7 @@
         <v>25</v>
       </c>
       <c r="E43" s="7">
-        <v>63650509.380000003</v>
+        <v>0</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
@@ -2755,7 +2759,7 @@
         <v>26</v>
       </c>
       <c r="E50" s="7">
-        <v>7352855.3600000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2766,7 +2770,7 @@
         <v>25</v>
       </c>
       <c r="E51" s="7">
-        <v>5320544.12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2807,7 +2811,7 @@
       <c r="D55" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="40">
+      <c r="E55" s="36">
         <v>0</v>
       </c>
     </row>
@@ -2818,7 +2822,7 @@
       <c r="D56" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="45">
+      <c r="E56" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2839,7 +2843,7 @@
         <v>26</v>
       </c>
       <c r="E58" s="7">
-        <v>16504650.689999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2850,7 +2854,7 @@
         <v>25</v>
       </c>
       <c r="E59" s="7">
-        <v>183698786.44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -2860,7 +2864,7 @@
       <c r="D60" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E60" s="44">
+      <c r="E60" s="40">
         <v>0</v>
       </c>
     </row>
@@ -2881,7 +2885,7 @@
         <v>26</v>
       </c>
       <c r="E62" s="7">
-        <v>8123744.0300000003</v>
+        <v>0</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
@@ -2895,7 +2899,7 @@
         <v>25</v>
       </c>
       <c r="E63" s="7">
-        <v>9624142.1300000008</v>
+        <v>0</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
@@ -2929,7 +2933,7 @@
         <v>26</v>
       </c>
       <c r="E66" s="7">
-        <v>8104195.3799999999</v>
+        <v>0</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
@@ -2945,7 +2949,7 @@
         <v>25</v>
       </c>
       <c r="E67" s="7">
-        <v>1016946.1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
@@ -3031,7 +3035,7 @@
       <c r="D75" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E75" s="40">
+      <c r="E75" s="36">
         <v>0</v>
       </c>
     </row>
@@ -3042,7 +3046,7 @@
       <c r="D76" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E76" s="47">
+      <c r="E76" s="43">
         <v>0</v>
       </c>
     </row>
@@ -3074,7 +3078,7 @@
       <c r="D79" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E79" s="40">
+      <c r="E79" s="36">
         <v>0</v>
       </c>
     </row>
@@ -3201,7 +3205,7 @@
         <v>14</v>
       </c>
       <c r="E91" s="7">
-        <v>274133.28999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3211,7 +3215,7 @@
       <c r="D92" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E92" s="45">
+      <c r="E92" s="41">
         <v>0</v>
       </c>
     </row>
@@ -3222,7 +3226,7 @@
       <c r="D93" s="8"/>
       <c r="E93" s="17">
         <f>SUM(E41:E92)</f>
-        <v>416551846.00000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3278,7 +3282,7 @@
       <c r="D98" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E98" s="40">
+      <c r="E98" s="36">
         <v>0</v>
       </c>
     </row>
@@ -3332,7 +3336,7 @@
       <c r="D104" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E104" s="44">
+      <c r="E104" s="40">
         <v>0</v>
       </c>
     </row>
@@ -3410,7 +3414,7 @@
       <c r="D112" s="2"/>
       <c r="E112" s="1">
         <f>SUM(E93,E111)</f>
-        <v>416551846.00000006</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3430,7 +3434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3C293A-74BB-4EAC-AF01-BCAF665D7CEB}">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E109" activeCellId="29" sqref="E10 E15 E20 E23 E28 E32 E41 E45 E49 E53 E57 E61 E65 E69 E73 E74 E77 E80 E83 E86 E89 E94 E95 E97 E99 E101 E103 E105 E107 E109"/>
     </sheetView>
   </sheetViews>
@@ -3444,307 +3448,307 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
+      <c r="A1" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="62" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
+      <c r="A4" s="62"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="62"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
       <c r="H5" s="32"/>
       <c r="I5" s="32"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="48"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="52" t="s">
+      <c r="B6" s="62"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="64" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="53"/>
+      <c r="A7" s="62"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="65"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="55"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="47"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50" t="s">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="55"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="47"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50" t="s">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="44"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="48">
         <v>693008.07</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50" t="s">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="48">
         <v>7955506.9699999997</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50" t="s">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="57">
+      <c r="E13" s="49">
         <v>75217.320000000007</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="50"/>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="50"/>
+      <c r="D14" s="44"/>
       <c r="E14" s="25">
         <f>SUM(E11:E13)</f>
         <v>8723732.3599999994</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="50"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="50"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50" t="s">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="48">
         <v>2560623.9300000002</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50" t="s">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="56">
+      <c r="E17" s="48">
         <v>12868353.91</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="50"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="50" t="s">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="56">
+      <c r="E18" s="48">
         <v>5339.73</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50" t="s">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="50"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="25">
         <f>SUM(E16:E18)</f>
         <v>15434317.57</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="50" t="s">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50" t="s">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="56">
+      <c r="D21" s="44"/>
+      <c r="E21" s="48">
         <v>419666830</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50" t="s">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="56">
+      <c r="D22" s="44"/>
+      <c r="E22" s="48">
         <v>261665.88</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50" t="s">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="50"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50" t="s">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="42">
+      <c r="E24" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50" t="s">
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="56">
+      <c r="E25" s="48">
         <v>650293.73</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50" t="s">
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="40">
+      <c r="E26" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="50"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50" t="s">
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="50"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50" t="s">
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="50"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="50"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50" t="s">
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44" t="s">
         <v>38</v>
       </c>
       <c r="E29" s="7">
@@ -3752,52 +3756,52 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="50"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50" t="s">
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="42">
+      <c r="E30" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="50"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50" t="s">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="43">
+      <c r="D31" s="44"/>
+      <c r="E31" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="50"/>
-      <c r="C32" s="50" t="s">
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="50"/>
+      <c r="D32" s="44"/>
       <c r="E32" s="9"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="50"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50" t="s">
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="44">
+      <c r="E33" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="50"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50" t="s">
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44" t="s">
         <v>33</v>
       </c>
       <c r="E34" s="7">
@@ -3805,10 +3809,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="50"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50" t="s">
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44" t="s">
         <v>32</v>
       </c>
       <c r="E35" s="10">
@@ -3816,109 +3820,109 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="50"/>
-      <c r="B36" s="50" t="s">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="56">
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="48">
         <v>134564635.53</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
-      <c r="B37" s="54" t="s">
+      <c r="A37" s="44"/>
+      <c r="B37" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
       <c r="E37" s="25">
         <f>SUM(E14,E19,E21:E36)</f>
         <v>579301475.07000005</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="50"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
+      <c r="A38" s="44"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
       <c r="E38" s="24"/>
     </row>
     <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="54"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
       <c r="E39" s="14"/>
     </row>
     <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
       <c r="E40" s="14"/>
     </row>
     <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="50"/>
-      <c r="B41" s="54" t="s">
+      <c r="A41" s="44"/>
+      <c r="B41" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
       <c r="E41" s="9"/>
     </row>
     <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="50"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50" t="s">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E42" s="56">
+      <c r="E42" s="48">
         <v>84186713.340000004</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="50"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50" t="s">
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="56">
+      <c r="E43" s="48">
         <v>135985125.53</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="50"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" s="56">
+      <c r="A44" s="44"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="48">
         <v>11056286.1</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
-      <c r="B45" s="54" t="s">
+      <c r="A45" s="44"/>
+      <c r="B45" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
       <c r="E45" s="9"/>
     </row>
     <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="59"/>
-      <c r="D46" s="50" t="s">
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="44" t="s">
         <v>26</v>
       </c>
       <c r="E46" s="7">
@@ -3926,10 +3930,10 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="50"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50" t="s">
+      <c r="A47" s="44"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44" t="s">
         <v>25</v>
       </c>
       <c r="E47" s="7">
@@ -3937,10 +3941,10 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="50"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50" t="s">
+      <c r="A48" s="44"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E48" s="7">
@@ -3948,41 +3952,41 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="50"/>
-      <c r="B49" s="54" t="s">
+      <c r="A49" s="44"/>
+      <c r="B49" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
       <c r="E49" s="10"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="60"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="50" t="s">
+      <c r="A50" s="52"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="52"/>
+      <c r="D50" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="56">
+      <c r="E50" s="48">
         <v>14262423.689999999</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="50"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50" t="s">
+      <c r="A51" s="44"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="56">
+      <c r="E51" s="48">
         <v>756418.16</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="50"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50" t="s">
+      <c r="A52" s="44"/>
+      <c r="B52" s="44"/>
+      <c r="C52" s="44"/>
+      <c r="D52" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E52" s="7">
@@ -3990,19 +3994,19 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="50"/>
-      <c r="B53" s="54" t="s">
+      <c r="A53" s="44"/>
+      <c r="B53" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
       <c r="E53" s="10"/>
     </row>
     <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="50"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
-      <c r="D54" s="50" t="s">
+      <c r="A54" s="44"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44" t="s">
         <v>26</v>
       </c>
       <c r="E54" s="7">
@@ -4010,105 +4014,105 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="50"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50" t="s">
+      <c r="A55" s="44"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="40">
+      <c r="E55" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="50"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56" s="45">
+      <c r="A56" s="44"/>
+      <c r="B56" s="44"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="50"/>
-      <c r="B57" s="54" t="s">
+      <c r="A57" s="44"/>
+      <c r="B57" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
+      <c r="C57" s="44"/>
+      <c r="D57" s="44"/>
       <c r="E57" s="22"/>
     </row>
     <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="50"/>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="50" t="s">
+      <c r="A58" s="44"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="44"/>
+      <c r="D58" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E58" s="44">
+      <c r="E58" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="50"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50" t="s">
+      <c r="A59" s="44"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="44"/>
+      <c r="D59" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E59" s="46">
+      <c r="E59" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="50"/>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="E60" s="44">
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
+      <c r="C60" s="44"/>
+      <c r="D60" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="50"/>
-      <c r="B61" s="54" t="s">
+      <c r="A61" s="44"/>
+      <c r="B61" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
+      <c r="C61" s="44"/>
+      <c r="D61" s="44"/>
       <c r="E61" s="22"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="50"/>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50" t="s">
+      <c r="A62" s="44"/>
+      <c r="B62" s="44"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E62" s="56">
+      <c r="E62" s="48">
         <v>2922659.4</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="50"/>
-      <c r="B63" s="54"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50" t="s">
+      <c r="A63" s="44"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="56">
+      <c r="E63" s="48">
         <v>597096.95999999996</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="50"/>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="50" t="s">
+      <c r="A64" s="44"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E64" s="7">
@@ -4116,41 +4120,41 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="50"/>
-      <c r="B65" s="54" t="s">
+      <c r="A65" s="44"/>
+      <c r="B65" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C65" s="50"/>
-      <c r="D65" s="50"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="44"/>
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="50"/>
-      <c r="B66" s="50"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="50" t="s">
+      <c r="A66" s="44"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="E66" s="56">
+      <c r="E66" s="48">
         <v>31729065.329999998</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="50"/>
-      <c r="B67" s="50"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="50" t="s">
+      <c r="A67" s="44"/>
+      <c r="B67" s="44"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="E67" s="56">
+      <c r="E67" s="48">
         <v>5991231.4100000001</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="50"/>
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="50" t="s">
+      <c r="A68" s="44"/>
+      <c r="B68" s="44"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E68" s="7">
@@ -4158,19 +4162,19 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="50"/>
-      <c r="B69" s="54" t="s">
+      <c r="A69" s="44"/>
+      <c r="B69" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C69" s="50"/>
-      <c r="D69" s="50"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
       <c r="E69" s="9"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="50"/>
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="50" t="s">
+      <c r="A70" s="44"/>
+      <c r="B70" s="44"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44" t="s">
         <v>26</v>
       </c>
       <c r="E70" s="14">
@@ -4178,10 +4182,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="50"/>
-      <c r="B71" s="50"/>
-      <c r="C71" s="50"/>
-      <c r="D71" s="50" t="s">
+      <c r="A71" s="44"/>
+      <c r="B71" s="44"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="44" t="s">
         <v>25</v>
       </c>
       <c r="E71" s="14">
@@ -4189,10 +4193,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="50"/>
-      <c r="B72" s="50"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50" t="s">
+      <c r="A72" s="44"/>
+      <c r="B72" s="44"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E72" s="21">
@@ -4200,125 +4204,125 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="50"/>
-      <c r="B73" s="54" t="s">
+      <c r="A73" s="44"/>
+      <c r="B73" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="44"/>
       <c r="E73" s="9"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="50"/>
-      <c r="B74" s="50"/>
-      <c r="C74" s="50" t="s">
+      <c r="A74" s="44"/>
+      <c r="B74" s="44"/>
+      <c r="C74" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="50"/>
+      <c r="D74" s="44"/>
       <c r="E74" s="14"/>
     </row>
     <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="50"/>
-      <c r="B75" s="50"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50" t="s">
+      <c r="A75" s="44"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="E75" s="56">
+      <c r="E75" s="48">
         <v>15785704.869999999</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="50"/>
-      <c r="B76" s="50"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50" t="s">
+      <c r="A76" s="44"/>
+      <c r="B76" s="44"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="E76" s="47">
+      <c r="E76" s="43">
         <v>54157654.939999998</v>
       </c>
-      <c r="F76" s="56"/>
+      <c r="F76" s="48"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A77" s="50"/>
-      <c r="B77" s="50"/>
-      <c r="C77" s="61" t="s">
+      <c r="A77" s="44"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D77" s="50"/>
+      <c r="D77" s="44"/>
       <c r="E77" s="14"/>
-      <c r="F77" s="56"/>
+      <c r="F77" s="48"/>
     </row>
     <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A78" s="50"/>
-      <c r="B78" s="50"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="50" t="s">
+      <c r="A78" s="44"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E78" s="56">
+      <c r="E78" s="48">
         <v>5035592.47</v>
       </c>
-      <c r="F78" s="56"/>
+      <c r="F78" s="48"/>
     </row>
     <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="50"/>
-      <c r="B79" s="50"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="50" t="s">
+      <c r="A79" s="44"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
+      <c r="D79" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E79" s="56">
+      <c r="E79" s="48">
         <v>4740000</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A80" s="50"/>
-      <c r="B80" s="50"/>
-      <c r="C80" s="50" t="s">
+      <c r="A80" s="44"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D80" s="50"/>
+      <c r="D80" s="44"/>
       <c r="E80" s="15"/>
     </row>
     <row r="81" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A81" s="50"/>
-      <c r="B81" s="50"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="61" t="s">
+      <c r="A81" s="44"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
+      <c r="D81" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="E81" s="56">
+      <c r="E81" s="48">
         <v>16567965.16</v>
       </c>
-      <c r="F81" s="56"/>
+      <c r="F81" s="48"/>
     </row>
     <row r="82" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="50"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="61" t="s">
+      <c r="A82" s="44"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
+      <c r="D82" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="E82" s="56">
+      <c r="E82" s="48">
         <v>3550000</v>
       </c>
-      <c r="F82" s="56"/>
+      <c r="F82" s="48"/>
     </row>
     <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="50"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="50" t="s">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="D83" s="50"/>
+      <c r="D83" s="44"/>
     </row>
     <row r="84" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="50"/>
-      <c r="B84" s="50"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50" t="s">
+      <c r="A84" s="44"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44" t="s">
         <v>14</v>
       </c>
       <c r="E84" s="18">
@@ -4326,10 +4330,10 @@
       </c>
     </row>
     <row r="85" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A85" s="50"/>
-      <c r="B85" s="50"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50" t="s">
+      <c r="A85" s="44"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="44"/>
+      <c r="D85" s="44" t="s">
         <v>13</v>
       </c>
       <c r="E85" s="18">
@@ -4337,19 +4341,19 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A86" s="50"/>
-      <c r="B86" s="50"/>
-      <c r="C86" s="50" t="s">
+      <c r="A86" s="44"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D86" s="50"/>
+      <c r="D86" s="44"/>
       <c r="E86" s="14"/>
     </row>
     <row r="87" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A87" s="50"/>
-      <c r="B87" s="50"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50" t="s">
+      <c r="A87" s="44"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44" t="s">
         <v>14</v>
       </c>
       <c r="E87" s="7">
@@ -4357,10 +4361,10 @@
       </c>
     </row>
     <row r="88" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A88" s="50"/>
-      <c r="B88" s="50"/>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50" t="s">
+      <c r="A88" s="44"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44" t="s">
         <v>13</v>
       </c>
       <c r="E88" s="7">
@@ -4368,19 +4372,19 @@
       </c>
     </row>
     <row r="89" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="50"/>
-      <c r="B89" s="50"/>
-      <c r="C89" s="50" t="s">
+      <c r="A89" s="44"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D89" s="50"/>
+      <c r="D89" s="44"/>
       <c r="E89" s="14"/>
     </row>
     <row r="90" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A90" s="50"/>
-      <c r="B90" s="50"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50" t="s">
+      <c r="A90" s="44"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="44"/>
+      <c r="D90" s="44" t="s">
         <v>15</v>
       </c>
       <c r="E90" s="7">
@@ -4388,106 +4392,106 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="50"/>
-      <c r="B91" s="50"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50" t="s">
+      <c r="A91" s="44"/>
+      <c r="B91" s="44"/>
+      <c r="C91" s="44"/>
+      <c r="D91" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="E91" s="56">
+      <c r="E91" s="48">
         <v>1437740.62</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A92" s="50"/>
-      <c r="B92" s="50"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50" t="s">
+      <c r="A92" s="44"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="44"/>
+      <c r="D92" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="E92" s="57">
+      <c r="E92" s="49">
         <v>114568496.95</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A93" s="54" t="s">
+      <c r="A93" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D93" s="50"/>
+      <c r="D93" s="44"/>
       <c r="E93" s="17">
         <f>SUM(E41:E92)</f>
         <v>503330174.93000007</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="54" t="s">
+      <c r="A94" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B94" s="50"/>
-      <c r="C94" s="54"/>
-      <c r="D94" s="61"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="46"/>
+      <c r="D94" s="53"/>
       <c r="E94" s="14"/>
     </row>
     <row r="95" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="50"/>
-      <c r="B95" s="54" t="s">
+      <c r="A95" s="44"/>
+      <c r="B95" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C95" s="50"/>
-      <c r="D95" s="50"/>
+      <c r="C95" s="44"/>
+      <c r="D95" s="44"/>
       <c r="E95" s="15"/>
-      <c r="H95" s="62"/>
-      <c r="I95" s="55"/>
+      <c r="H95" s="54"/>
+      <c r="I95" s="47"/>
     </row>
     <row r="96" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="50"/>
-      <c r="B96" s="50"/>
-      <c r="C96" s="50"/>
-      <c r="D96" s="50" t="s">
+      <c r="A96" s="44"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="44"/>
+      <c r="D96" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E96" s="7">
         <v>0</v>
       </c>
-      <c r="F96" s="62"/>
-      <c r="G96" s="50"/>
-      <c r="I96" s="55"/>
+      <c r="F96" s="54"/>
+      <c r="G96" s="44"/>
+      <c r="I96" s="47"/>
     </row>
     <row r="97" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="50"/>
-      <c r="B97" s="54" t="s">
+      <c r="A97" s="44"/>
+      <c r="B97" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
+      <c r="C97" s="44"/>
+      <c r="D97" s="44"/>
       <c r="E97" s="14"/>
-      <c r="F97" s="62"/>
-      <c r="G97" s="50"/>
-      <c r="H97" s="62"/>
-      <c r="I97" s="55"/>
+      <c r="F97" s="54"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="54"/>
+      <c r="I97" s="47"/>
     </row>
     <row r="98" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B98" s="50"/>
-      <c r="C98" s="50"/>
-      <c r="D98" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="E98" s="40">
+      <c r="B98" s="44"/>
+      <c r="C98" s="44"/>
+      <c r="D98" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E98" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="54" t="s">
+      <c r="B99" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
+      <c r="C99" s="44"/>
+      <c r="D99" s="44"/>
       <c r="E99" s="9"/>
     </row>
     <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="50"/>
-      <c r="C100" s="50"/>
-      <c r="D100" s="50" t="s">
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E100" s="7">
@@ -4495,17 +4499,17 @@
       </c>
     </row>
     <row r="101" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="54" t="s">
+      <c r="B101" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C101" s="50"/>
-      <c r="D101" s="50"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="44"/>
       <c r="E101" s="9"/>
     </row>
     <row r="102" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B102" s="50"/>
-      <c r="C102" s="59"/>
-      <c r="D102" s="50" t="s">
+      <c r="B102" s="44"/>
+      <c r="C102" s="51"/>
+      <c r="D102" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E102" s="10">
@@ -4513,34 +4517,34 @@
       </c>
     </row>
     <row r="103" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B103" s="54" t="s">
+      <c r="B103" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C103" s="50"/>
-      <c r="D103" s="50"/>
+      <c r="C103" s="44"/>
+      <c r="D103" s="44"/>
       <c r="E103" s="9"/>
     </row>
     <row r="104" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B104" s="50"/>
-      <c r="C104" s="50"/>
-      <c r="D104" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="E104" s="44">
+      <c r="B104" s="44"/>
+      <c r="C104" s="44"/>
+      <c r="D104" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="E104" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B105" s="54" t="s">
+      <c r="B105" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
+      <c r="C105" s="44"/>
+      <c r="D105" s="44"/>
     </row>
     <row r="106" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B106" s="50"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50" t="s">
+      <c r="B106" s="44"/>
+      <c r="C106" s="44"/>
+      <c r="D106" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E106" s="9">
@@ -4548,17 +4552,17 @@
       </c>
     </row>
     <row r="107" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B107" s="54" t="s">
+      <c r="B107" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
+      <c r="C107" s="44"/>
+      <c r="D107" s="44"/>
       <c r="E107" s="9"/>
     </row>
     <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B108" s="50"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50" t="s">
+      <c r="B108" s="44"/>
+      <c r="C108" s="44"/>
+      <c r="D108" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E108" s="7">
@@ -4566,27 +4570,27 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A109" s="54"/>
-      <c r="B109" s="54" t="s">
+      <c r="A109" s="46"/>
+      <c r="B109" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C109" s="50"/>
-      <c r="D109" s="50"/>
+      <c r="C109" s="44"/>
+      <c r="D109" s="44"/>
       <c r="E109" s="9"/>
     </row>
     <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B110" s="50"/>
-      <c r="C110" s="50"/>
-      <c r="D110" s="50" t="s">
+      <c r="B110" s="44"/>
+      <c r="C110" s="44"/>
+      <c r="D110" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E110" s="7">
         <v>0</v>
       </c>
-      <c r="F110" s="63"/>
+      <c r="F110" s="55"/>
     </row>
     <row r="111" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A111" s="54" t="s">
+      <c r="A111" s="46" t="s">
         <v>1</v>
       </c>
       <c r="E111" s="4">
@@ -4595,12 +4599,12 @@
       </c>
     </row>
     <row r="112" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="B112" s="65"/>
-      <c r="C112" s="65"/>
-      <c r="D112" s="65"/>
+      <c r="A112" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="57"/>
+      <c r="C112" s="57"/>
+      <c r="D112" s="57"/>
       <c r="E112" s="1">
         <f>SUM(E93,E111)</f>
         <v>503330174.93000007</v>

</xml_diff>